<commit_message>
Correction "corrigée" du Sprint 2
</commit_message>
<xml_diff>
--- a/Equipe102.xlsx
+++ b/Equipe102.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27605"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nikolay\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="454" documentId="13_ncr:1_{DBEB54B7-8C9A-40C2-9BEC-806A0CAE1E88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3618203C-20EF-4F85-834E-B1EDCCA49486}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{A5B64CA1-2FF6-4C83-9253-961CF1308BF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3461,13 +3461,13 @@
     </xf>
   </cellXfs>
   <cellStyles count="7">
-    <cellStyle name="40% - Accent1" xfId="4" builtinId="31"/>
-    <cellStyle name="40% - Accent2" xfId="5" builtinId="35"/>
-    <cellStyle name="40% - Accent3" xfId="6" builtinId="39"/>
-    <cellStyle name="Explanatory Text" xfId="2" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="40 % - Accent1" xfId="4" builtinId="31"/>
+    <cellStyle name="40 % - Accent2" xfId="5" builtinId="35"/>
+    <cellStyle name="40 % - Accent3" xfId="6" builtinId="39"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Output" xfId="3" builtinId="21"/>
-    <cellStyle name="Percent" xfId="1" builtinId="5"/>
+    <cellStyle name="Pourcentage" xfId="1" builtinId="5"/>
+    <cellStyle name="Sortie" xfId="3" builtinId="21"/>
+    <cellStyle name="Texte explicatif" xfId="2" builtinId="53" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -3920,11 +3920,11 @@
       </c>
       <c r="C5" s="110">
         <f>'Assurance Qualité'!F59</f>
-        <v>0.66650000000000009</v>
+        <v>0.6915</v>
       </c>
       <c r="D5" s="110">
         <f t="shared" ref="D5:D6" si="1">B5*0.6+C5*0.4 - 0.1*E5</f>
-        <v>0.81072500000000003</v>
+        <v>0.82072499999999993</v>
       </c>
       <c r="E5" s="111"/>
       <c r="F5" s="112">
@@ -3932,7 +3932,7 @@
       </c>
       <c r="G5" s="113">
         <f t="shared" si="0"/>
-        <v>20.268125000000001</v>
+        <v>20.518124999999998</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -3988,8 +3988,8 @@
   <sheetPr codeName="Sheet7"/>
   <dimension ref="A2:Q59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B47" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F45" sqref="F45"/>
+    <sheetView tabSelected="1" topLeftCell="B37" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K45" sqref="K45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -4329,7 +4329,7 @@
       <c r="L13" s="5"/>
       <c r="M13" s="5"/>
     </row>
-    <row r="14" spans="1:17" ht="60.75">
+    <row r="14" spans="1:17" ht="96" customHeight="1">
       <c r="A14" s="23" t="s">
         <v>31</v>
       </c>
@@ -4383,7 +4383,7 @@
         <v>37</v>
       </c>
       <c r="F15" s="86">
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="G15" s="90">
         <f t="shared" si="0"/>
@@ -4487,7 +4487,7 @@
       <c r="E18" s="49"/>
       <c r="F18" s="50">
         <f>SUMPRODUCT(F13:F17,G13:G17)</f>
-        <v>11.25</v>
+        <v>11.75</v>
       </c>
       <c r="G18" s="51">
         <f>SUM(G13:G17)</f>
@@ -4688,7 +4688,7 @@
       <c r="L24" s="5"/>
       <c r="M24" s="5"/>
     </row>
-    <row r="25" spans="1:17" ht="213">
+    <row r="25" spans="1:17" ht="137.25">
       <c r="A25" s="23" t="s">
         <v>54</v>
       </c>
@@ -4814,7 +4814,7 @@
       <c r="L28" s="9"/>
       <c r="M28" s="4"/>
     </row>
-    <row r="29" spans="1:17" ht="121.5">
+    <row r="29" spans="1:17" ht="76.5">
       <c r="A29" s="31" t="s">
         <v>62</v>
       </c>
@@ -5368,7 +5368,7 @@
         <v>107</v>
       </c>
       <c r="F45" s="86">
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
       <c r="G45" s="87">
         <f t="shared" si="4"/>
@@ -5388,7 +5388,7 @@
       <c r="L45" s="5"/>
       <c r="M45" s="5"/>
     </row>
-    <row r="46" spans="1:13" ht="183">
+    <row r="46" spans="1:13" ht="152.25">
       <c r="A46" s="23" t="s">
         <v>109</v>
       </c>
@@ -5509,7 +5509,7 @@
       <c r="E49" s="59"/>
       <c r="F49" s="70">
         <f>SUMPRODUCT(F40:F48,G40:G48)</f>
-        <v>24.5</v>
+        <v>26.5</v>
       </c>
       <c r="G49" s="51">
         <f>SUM(G40:G48)</f>
@@ -5784,7 +5784,7 @@
       <c r="E58" s="26"/>
       <c r="F58" s="35">
         <f>F11+F18+F22+F27+F32+F38+F49+F56</f>
-        <v>66.650000000000006</v>
+        <v>69.150000000000006</v>
       </c>
       <c r="G58" s="27">
         <f>G11+G18+G22+G27+G32+G38+G49+G56</f>
@@ -5816,7 +5816,7 @@
       <c r="E59" s="237"/>
       <c r="F59" s="238">
         <f>F58/G58</f>
-        <v>0.66650000000000009</v>
+        <v>0.6915</v>
       </c>
       <c r="G59" s="239"/>
       <c r="H59" s="240"/>
@@ -5903,7 +5903,7 @@
   <sheetPr codeName="Sheet8"/>
   <dimension ref="A2:G44"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A14" workbookViewId="0">
       <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>

</xml_diff>